<commit_message>
Added CartPage, CartTest and tesng.xml
</commit_message>
<xml_diff>
--- a/data/pet-store-data.xlsx
+++ b/data/pet-store-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="721">
   <si>
     <t>ITEM_ID</t>
   </si>
@@ -2029,6 +2029,156 @@
   </si>
   <si>
     <t>5030a02</t>
+  </si>
+  <si>
+    <t>64cda32</t>
+  </si>
+  <si>
+    <t>6557686</t>
+  </si>
+  <si>
+    <t>5df29c9</t>
+  </si>
+  <si>
+    <t>6363e33</t>
+  </si>
+  <si>
+    <t>d3c4ef7</t>
+  </si>
+  <si>
+    <t>c054e5e</t>
+  </si>
+  <si>
+    <t>f96a497</t>
+  </si>
+  <si>
+    <t>db7cfd0</t>
+  </si>
+  <si>
+    <t>786f3d7</t>
+  </si>
+  <si>
+    <t>7633f2f</t>
+  </si>
+  <si>
+    <t>050c98d</t>
+  </si>
+  <si>
+    <t>3a47835</t>
+  </si>
+  <si>
+    <t>c6e056b</t>
+  </si>
+  <si>
+    <t>6af4d48</t>
+  </si>
+  <si>
+    <t>78f58cb</t>
+  </si>
+  <si>
+    <t>c11c197</t>
+  </si>
+  <si>
+    <t>8b2fc9b</t>
+  </si>
+  <si>
+    <t>13eeabc</t>
+  </si>
+  <si>
+    <t>561f00d</t>
+  </si>
+  <si>
+    <t>ab16b44</t>
+  </si>
+  <si>
+    <t>4f1bb5f</t>
+  </si>
+  <si>
+    <t>b2c317c</t>
+  </si>
+  <si>
+    <t>88ff7ce</t>
+  </si>
+  <si>
+    <t>81631aa</t>
+  </si>
+  <si>
+    <t>51e0737</t>
+  </si>
+  <si>
+    <t>6b9b71d</t>
+  </si>
+  <si>
+    <t>48849e1</t>
+  </si>
+  <si>
+    <t>9265672</t>
+  </si>
+  <si>
+    <t>1234223</t>
+  </si>
+  <si>
+    <t>7bcd4b3</t>
+  </si>
+  <si>
+    <t>2a17c26</t>
+  </si>
+  <si>
+    <t>233f76d</t>
+  </si>
+  <si>
+    <t>bf8a9d9</t>
+  </si>
+  <si>
+    <t>a112f10</t>
+  </si>
+  <si>
+    <t>9ad27a3</t>
+  </si>
+  <si>
+    <t>0f2670d</t>
+  </si>
+  <si>
+    <t>8e494eb</t>
+  </si>
+  <si>
+    <t>3e67820</t>
+  </si>
+  <si>
+    <t>cd1beb3</t>
+  </si>
+  <si>
+    <t>240d155</t>
+  </si>
+  <si>
+    <t>e131504</t>
+  </si>
+  <si>
+    <t>896814c</t>
+  </si>
+  <si>
+    <t>118359f</t>
+  </si>
+  <si>
+    <t>76cbc16</t>
+  </si>
+  <si>
+    <t>a9bb6e5</t>
+  </si>
+  <si>
+    <t>5c5f64f</t>
+  </si>
+  <si>
+    <t>e48e2d5</t>
+  </si>
+  <si>
+    <t>617054d</t>
+  </si>
+  <si>
+    <t>9e6fca1</t>
+  </si>
+  <si>
+    <t>184222d</t>
   </si>
 </sst>
 </file>
@@ -2672,7 +2822,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>14</v>
@@ -2710,7 +2860,7 @@
     </row>
     <row r="3" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>619</v>
+        <v>672</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
@@ -2748,7 +2898,7 @@
     </row>
     <row r="4" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>620</v>
+        <v>673</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>33</v>
@@ -2786,7 +2936,7 @@
     </row>
     <row r="5" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>621</v>
+        <v>674</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>42</v>
@@ -2824,7 +2974,7 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>622</v>
+        <v>675</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>51</v>
@@ -2862,7 +3012,7 @@
     </row>
     <row r="7" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>623</v>
+        <v>676</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>60</v>
@@ -2900,7 +3050,7 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>624</v>
+        <v>677</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>69</v>
@@ -2938,7 +3088,7 @@
     </row>
     <row r="9" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>625</v>
+        <v>678</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>78</v>
@@ -2976,7 +3126,7 @@
     </row>
     <row r="10" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>626</v>
+        <v>679</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>87</v>
@@ -3014,7 +3164,7 @@
     </row>
     <row r="11" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>627</v>
+        <v>680</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>96</v>
@@ -3052,7 +3202,7 @@
     </row>
     <row r="12" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>628</v>
+        <v>681</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>105</v>
@@ -3090,7 +3240,7 @@
     </row>
     <row r="13" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>629</v>
+        <v>682</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>114</v>
@@ -3128,7 +3278,7 @@
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>630</v>
+        <v>683</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>123</v>
@@ -3166,7 +3316,7 @@
     </row>
     <row r="15" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>631</v>
+        <v>684</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>131</v>
@@ -3204,7 +3354,7 @@
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>632</v>
+        <v>685</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>139</v>
@@ -3242,7 +3392,7 @@
     </row>
     <row r="17" spans="1:12" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>633</v>
+        <v>686</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>148</v>
@@ -3280,7 +3430,7 @@
     </row>
     <row r="18" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>634</v>
+        <v>687</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>156</v>
@@ -3318,7 +3468,7 @@
     </row>
     <row r="19" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>635</v>
+        <v>688</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>165</v>
@@ -3356,7 +3506,7 @@
     </row>
     <row r="20" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>636</v>
+        <v>689</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>173</v>
@@ -3394,7 +3544,7 @@
     </row>
     <row r="21" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>637</v>
+        <v>690</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>181</v>
@@ -3432,7 +3582,7 @@
     </row>
     <row r="22" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>638</v>
+        <v>691</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>190</v>
@@ -3470,7 +3620,7 @@
     </row>
     <row r="23" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>639</v>
+        <v>692</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>199</v>
@@ -3508,7 +3658,7 @@
     </row>
     <row r="24" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>640</v>
+        <v>693</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>207</v>
@@ -3546,7 +3696,7 @@
     </row>
     <row r="25" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>641</v>
+        <v>694</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>216</v>
@@ -3584,7 +3734,7 @@
     </row>
     <row r="26" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>642</v>
+        <v>695</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>225</v>
@@ -3622,7 +3772,7 @@
     </row>
     <row r="27" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>643</v>
+        <v>696</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>234</v>
@@ -3660,7 +3810,7 @@
     </row>
     <row r="28" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>644</v>
+        <v>697</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>243</v>
@@ -3698,7 +3848,7 @@
     </row>
     <row r="29" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>645</v>
+        <v>698</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>251</v>
@@ -3736,7 +3886,7 @@
     </row>
     <row r="30" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>646</v>
+        <v>699</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>259</v>
@@ -3774,7 +3924,7 @@
     </row>
     <row r="31" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>647</v>
+        <v>700</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>268</v>
@@ -3812,7 +3962,7 @@
     </row>
     <row r="32" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>648</v>
+        <v>701</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>276</v>
@@ -3850,7 +4000,7 @@
     </row>
     <row r="33" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>649</v>
+        <v>702</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>284</v>
@@ -3888,7 +4038,7 @@
     </row>
     <row r="34" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>650</v>
+        <v>703</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>292</v>
@@ -3926,7 +4076,7 @@
     </row>
     <row r="35" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>651</v>
+        <v>704</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>301</v>
@@ -3964,7 +4114,7 @@
     </row>
     <row r="36" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>652</v>
+        <v>705</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>310</v>
@@ -4002,7 +4152,7 @@
     </row>
     <row r="37" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>653</v>
+        <v>706</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>319</v>
@@ -4040,7 +4190,7 @@
     </row>
     <row r="38" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>654</v>
+        <v>707</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>327</v>
@@ -4078,7 +4228,7 @@
     </row>
     <row r="39" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>655</v>
+        <v>708</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>336</v>
@@ -4116,7 +4266,7 @@
     </row>
     <row r="40" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>656</v>
+        <v>709</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>344</v>
@@ -4154,7 +4304,7 @@
     </row>
     <row r="41" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>657</v>
+        <v>710</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>352</v>
@@ -4192,7 +4342,7 @@
     </row>
     <row r="42" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>658</v>
+        <v>711</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>360</v>
@@ -4230,7 +4380,7 @@
     </row>
     <row r="43" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>659</v>
+        <v>712</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>368</v>
@@ -4268,7 +4418,7 @@
     </row>
     <row r="44" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>660</v>
+        <v>713</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>377</v>
@@ -4306,7 +4456,7 @@
     </row>
     <row r="45" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>661</v>
+        <v>714</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>386</v>
@@ -4344,7 +4494,7 @@
     </row>
     <row r="46" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>662</v>
+        <v>715</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>394</v>
@@ -4382,7 +4532,7 @@
     </row>
     <row r="47" spans="1:12" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>663</v>
+        <v>716</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>402</v>
@@ -4420,7 +4570,7 @@
     </row>
     <row r="48" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>664</v>
+        <v>717</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>410</v>
@@ -4458,7 +4608,7 @@
     </row>
     <row r="49" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>665</v>
+        <v>718</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>418</v>
@@ -4496,7 +4646,7 @@
     </row>
     <row r="50" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>666</v>
+        <v>719</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>427</v>
@@ -4534,7 +4684,7 @@
     </row>
     <row r="51" spans="1:12" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>667</v>
+        <v>720</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>436</v>

</xml_diff>